<commit_message>
updated bank details and site header color
</commit_message>
<xml_diff>
--- a/src/sourcefiles/Ashramam_Items_Donors.xlsx
+++ b/src/sourcefiles/Ashramam_Items_Donors.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
   <si>
     <t>SNO</t>
   </si>
@@ -359,6 +359,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -406,7 +409,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -441,7 +444,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -653,7 +656,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1175,12 +1178,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
-        <v>23</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>